<commit_message>
create import error ok
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Gia_Tri_Gia_Tang_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Gia_Tri_Gia_Tang_Import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\Template\ImportHoaDon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17921083-FA10-48ED-8D37-DF3B80132650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D895832F-A02C-4ADD-9781-8384B60C2F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hóa đơn giá trị gia tăng" sheetId="1" r:id="rId1"/>
     <sheet name="Nguyên tắc ghép dữ liệu" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="198">
   <si>
     <t>Số thứ tự hóa đơn (*)</t>
   </si>
@@ -636,9 +636,6 @@
     <t>Đơn vị</t>
   </si>
   <si>
-    <t>Đơn vị (*)</t>
-  </si>
-  <si>
     <t>Nhập Đơn vị lập hóa đơn</t>
   </si>
   <si>
@@ -651,7 +648,52 @@
 Nhập 4 nếu là Ghi chú/Diễn giải</t>
   </si>
   <si>
-    <t>HHDV4</t>
+    <t>NM3</t>
+  </si>
+  <si>
+    <t>NM4</t>
+  </si>
+  <si>
+    <t>NM5</t>
+  </si>
+  <si>
+    <t>NM6</t>
+  </si>
+  <si>
+    <t>NM7</t>
+  </si>
+  <si>
+    <t>NM9</t>
+  </si>
+  <si>
+    <t>NM10</t>
+  </si>
+  <si>
+    <t>HHDV3</t>
+  </si>
+  <si>
+    <t>HHDV6</t>
+  </si>
+  <si>
+    <t>HHDV7</t>
+  </si>
+  <si>
+    <t>HHDV9</t>
+  </si>
+  <si>
+    <t>HHDV11</t>
+  </si>
+  <si>
+    <t>HHDV12</t>
+  </si>
+  <si>
+    <t>HHDV16</t>
+  </si>
+  <si>
+    <t>HHDV17</t>
+  </si>
+  <si>
+    <t>HHDV18</t>
   </si>
 </sst>
 </file>
@@ -1202,91 +1244,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA64"/>
+  <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="R10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="26.5703125" style="1"/>
-    <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
-    <col min="4" max="8" width="26.5703125" style="1"/>
-    <col min="9" max="9" width="26.5703125" style="2"/>
-    <col min="10" max="26" width="26.5703125" style="1"/>
-    <col min="28" max="16384" width="26.5703125" style="1"/>
+    <col min="1" max="7" width="26.5703125" style="1"/>
+    <col min="8" max="8" width="26.5703125" style="2"/>
+    <col min="9" max="24" width="26.5703125" style="1"/>
+    <col min="26" max="16384" width="26.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:25" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>139</v>
       </c>
@@ -1294,149 +1334,137 @@
         <v>167</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>177</v>
+        <v>129</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>44</v>
+        <v>183</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>45</v>
+        <v>184</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>46</v>
+        <v>185</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>47</v>
+        <v>186</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>48</v>
+        <v>187</v>
       </c>
       <c r="L15" s="20" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="M15" s="20" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="O15" s="20" t="s">
-        <v>127</v>
+        <v>189</v>
       </c>
       <c r="P15" s="20" t="s">
-        <v>52</v>
+        <v>190</v>
       </c>
       <c r="Q15" s="20" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="R15" s="20" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="S15" s="20" t="s">
-        <v>56</v>
+        <v>193</v>
       </c>
       <c r="T15" s="20" t="s">
-        <v>58</v>
+        <v>194</v>
       </c>
       <c r="U15" s="20" t="s">
-        <v>60</v>
+        <v>195</v>
       </c>
       <c r="V15" s="20" t="s">
-        <v>61</v>
+        <v>196</v>
       </c>
       <c r="W15" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="X15" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y15" s="20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>160</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>179</v>
+      <c r="C16" s="26" t="s">
+        <v>101</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M16" s="26" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="N16" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="O16" s="26" t="s">
         <v>14</v>
       </c>
+      <c r="O16" s="27" t="s">
+        <v>165</v>
+      </c>
       <c r="P16" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q16" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="R16" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="S16" s="28" t="s">
+      <c r="Q16" s="28" t="s">
         <v>8</v>
       </c>
+      <c r="R16" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="S16" s="29" t="s">
+        <v>10</v>
+      </c>
       <c r="T16" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="U16" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="V16" s="29" t="s">
         <v>15</v>
       </c>
+      <c r="U16" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="V16" s="30" t="s">
+        <v>11</v>
+      </c>
       <c r="W16" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="X16" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y16" s="30" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1585,34 +1613,31 @@
       <c r="A64" s="18"/>
     </row>
   </sheetData>
-  <dataValidations count="27">
+  <dataValidations count="24">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Không nhập thông tin tại cột này" sqref="A16:A1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập số thứ tự của hóa đơn._x000a_Lưu ý: Mỗi số thứ tự sẽ tương ứng với 1 hóa đơn_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống." sqref="B16:B1048576" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Ngày hóa đơn." sqref="E16 E17:E1048576" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên người mua hàng" sqref="F17:F1048576 F16" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên khách hàng" sqref="G17:G1048576 G16" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Địa chỉ" sqref="H17:H1048576 H16" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã số thuế_x000a_Tối đa 14 ký tự" sqref="I17:I1048576 I16" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Hình thức thanh toán" sqref="J17:J1048576 J16" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Email người nhận hóa đơn._x000a_Nếu nhiều Email thì mỗi Email cách nhau bởi dấu &quot;;&quot;" sqref="K17:K1048576 K16" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số tài khoản ngân hàng" sqref="L17:L1048576 L16" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên ngân hàng" sqref="M17:M1048576 M16" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã loại tiền._x000a_Nếu để trống ngầm định là VND." sqref="N17:N1048576 N16" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ giá_x000a_Tối đa 15 ký tự" sqref="O17:O1048576 O16" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên hàng hóa, dịch vụ._x000a_Trường dữ liệu bắt buộc._x000a_Không để trống" sqref="P16 P17:P1048576" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn vị tính." sqref="R16:R17 R19:R1048576" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền thuế GTGT quy đổi của hóa đơn_x000a_Tối đa 15 ký tự" sqref="Y17:Y1048576 Y16" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền thuế GTGT của hóa đơn_x000a_Tối đa 15 ký tự" sqref="X17:X1048576 X16" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập % Thuế GTGT:_x000a_- 0: 0%_x000a_- 5: 5%_x000a_- 10: 10%_x000a_- KCT: Không chịu thuế_x000a_- KKKNT: Không kê khai nộp thuế_x000a_- KHAC: Khác" sqref="W17:W1048576 W16" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền quy đổi_x000a_Tối đa 15 ký tự" sqref="V17:V1048576 V16" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền_x000a_Tối đa 15 ký tự" sqref="U17:U1048576 U16" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn giá_x000a_Tối đa 15 ký tự" sqref="T17:T1048576 T16" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số lượng_x000a_Tối đa 15 ký tự" sqref="S17:S1048576 S16" xr:uid="{00000000-0002-0000-0000-000015000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã đơn vị lập hóa đơn._x000a_Lưu ý:_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống._x000a_Nhập theo danh mục đã tạo tại Danh mục/Cơ cấu tổ chức" sqref="C16:C1048576" xr:uid="{00000000-0002-0000-0000-000016000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã trường dữ liệu/Tiện ích tương ứng trên Hóa đơn Bách Khoa" sqref="C15:D15 E15:P15 R15:Y15" xr:uid="{00000000-0002-0000-0000-000017000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập Mã nhân viên bán hàng._x000a_Lưu ý:_x000a_Để trống nếu không thiết lập Tùy chọn/Quản lý nhân viên bán hàng trên hóa đơn._x000a_Nhập theo danh mục đã tạo tại Danh mục/Nhân viên" sqref="D16:D1048576" xr:uid="{00000000-0002-0000-0000-000018000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Tính chất." sqref="Q2 Q15" xr:uid="{30BB3401-499F-4DD0-9D31-C3AAA351A641}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tính chất._x000a_Nhập 1 hoặc để trống: Hàng hóa, dịch vụ._x000a_Nhập 2: Khuyến mại._x000a_Nhập 3: Chiết khấu thương mại._x000a_Nhập 4: Ghi chú/Diễn giải." sqref="Q16:Q1048576" xr:uid="{B530E0E4-F64E-4667-9780-8847C87A9E2E}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Ngày hóa đơn." sqref="D16 D17:D1048576" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên người mua hàng" sqref="E17:E1048576 E16" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên khách hàng" sqref="F17:F1048576 F16" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Địa chỉ" sqref="G17:G1048576 G16" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã số thuế_x000a_Tối đa 14 ký tự" sqref="H17:H1048576 H16" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Hình thức thanh toán" sqref="I17:I1048576 I16" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Email người nhận hóa đơn._x000a_Nếu nhiều Email thì mỗi Email cách nhau bởi dấu &quot;;&quot;" sqref="J17:J1048576 J16" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số tài khoản ngân hàng" sqref="K17:K1048576 K16" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên ngân hàng" sqref="L17:L1048576 L16" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã loại tiền._x000a_Nếu để trống ngầm định là VND." sqref="M17:M1048576 M16" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ giá_x000a_Tối đa 15 ký tự" sqref="N17:N1048576 N16" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên hàng hóa, dịch vụ._x000a_Trường dữ liệu bắt buộc._x000a_Không để trống" sqref="O16 O17:O1048576" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn vị tính." sqref="P16:P17 P19:P1048576" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền thuế GTGT quy đổi của hóa đơn_x000a_Tối đa 15 ký tự" sqref="W17:W1048576 W16" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền thuế GTGT của hóa đơn_x000a_Tối đa 15 ký tự" sqref="V17:V1048576 V16" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập % Thuế GTGT:_x000a_- 0: 0%_x000a_- 5: 5%_x000a_- 10: 10%_x000a_- KCT: Không chịu thuế_x000a_- KKKNT: Không kê khai nộp thuế_x000a_- KHAC: Khác" sqref="U17:U1048576 U16" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền quy đổi_x000a_Tối đa 15 ký tự" sqref="T17:T1048576 T16" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền_x000a_Tối đa 15 ký tự" sqref="S17:S1048576 S16" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn giá_x000a_Tối đa 15 ký tự" sqref="R17:R1048576 R16" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số lượng_x000a_Tối đa 15 ký tự" sqref="Q17:Q1048576 Q16" xr:uid="{00000000-0002-0000-0000-000015000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã trường dữ liệu/Tiện ích tương ứng trên Hóa đơn Bách Khoa" sqref="P15:W15 C15:O15" xr:uid="{00000000-0002-0000-0000-000017000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập Mã nhân viên bán hàng._x000a_Lưu ý:_x000a_Để trống nếu không thiết lập Tùy chọn/Quản lý nhân viên bán hàng trên hóa đơn._x000a_Nhập theo danh mục đã tạo tại Danh mục/Nhân viên" sqref="C16:C1048576" xr:uid="{00000000-0002-0000-0000-000018000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1681,7 +1706,7 @@
         <v>178</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1930,10 +1955,10 @@
         <v>53</v>
       </c>
       <c r="C25" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
dieu chinh so tien bang chu
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Gia_Tri_Gia_Tang_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Gia_Tri_Gia_Tang_Import.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\Template\ImportHoaDon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B628B77-9856-4E25-9A47-B21ADCC8574C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F4AFF1-502F-466B-A86F-1185A6915E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hóa đơn giá trị gia tăng" sheetId="1" r:id="rId1"/>
@@ -629,6 +629,7 @@
       <t xml:space="preserve">Nhập % Thuế GTGT:
 - 0: 0%
 - 5: 5%
+- 8: 8%
 - 10: 10%
 - KCT: Không chịu thuế
 - KKKNT: Không kê khai nộp thuế
@@ -1191,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1550,7 @@
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn vị tính." sqref="P16:P1048576" xr:uid="{00000000-0002-0000-0100-00000B000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền thuế GTGT quy đổi của hóa đơn_x000a_Tối đa 15 ký tự" sqref="Z16:Z1048576" xr:uid="{00000000-0002-0000-0100-00000C000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền thuế GTGT của hóa đơn_x000a_Tối đa 15 ký tự" sqref="Y16:Y1048576" xr:uid="{00000000-0002-0000-0100-00000D000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập % Thuế GTGT:_x000a_- 0: 0%_x000a_- 5: 5%_x000a_- 8: 8%_x000a_- 10: 10%_x000a_- KCT: Không chịu thuế_x000a_- KKKNT: Không kê khai nộp thuế_x000a_- AB.CD%: Khác (Trong đó: A, B, C, D là các số nguyên từ 0 đến 9)" sqref="X16:X1048576" xr:uid="{00000000-0002-0000-0100-00000E000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập % Thuế GTGT:_x000a_- 0: 0%_x000a_- 5: 5%_x000a_- 8: 8%_x000a_- 10: 10%_x000a_- KCT: Không chịu thuế_x000a_- KKKNT: Không kê khai nộp thuế_x000a_- AB.CD%: Khác. Trong đó: A, B, C, D là các số nguyên từ 0 đến 9._x000a_Ví dụ: 3,5% có thể nhập là 03.50% hoặc 03.5% hoặc 3.5% hoặc 3.50%" sqref="X16:X1048576" xr:uid="{00000000-0002-0000-0100-00000E000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền quy đổi_x000a_Tối đa 15 ký tự" sqref="T16:T1048576" xr:uid="{00000000-0002-0000-0100-00000F000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền_x000a_Tối đa 15 ký tự" sqref="S16" xr:uid="{00000000-0002-0000-0100-000010000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn giá_x000a_Tối đa 15 ký tự" sqref="R16:R1048576" xr:uid="{00000000-0002-0000-0100-000011000000}"/>
@@ -1575,8 +1576,8 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView showGridLines="0" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2025,7 +2026,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>38</v>
       </c>

</xml_diff>